<commit_message>
minor bug fixes & centraal data
</commit_message>
<xml_diff>
--- a/data/centraal_trees.xlsx
+++ b/data/centraal_trees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iris Reitsma\Documents\Master\jaar 2\stage\root_model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A38733-8901-4A75-94E8-ABAB18BBEDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736F22D3-7D21-4C1C-8831-95B13517C5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4A5EA58-55A2-4CF5-A20D-4EEE611D84CF}"/>
+    <workbookView xWindow="28680" yWindow="-6750" windowWidth="29040" windowHeight="15840" xr2:uid="{C4A5EA58-55A2-4CF5-A20D-4EEE611D84CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="82">
   <si>
     <t>Soortnaam_NL</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>POINT(52.379899 4.896057)</t>
+  </si>
+  <si>
+    <t>RD_X</t>
+  </si>
+  <si>
+    <t>RD_Y</t>
   </si>
 </sst>
 </file>
@@ -627,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC3DC2D-BDA2-41E6-89ED-F233956BF6EF}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,7 +649,7 @@
     <col min="19" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -701,8 +707,14 @@
       <c r="S1" t="s">
         <v>77</v>
       </c>
+      <c r="T1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>235853</v>
       </c>
@@ -760,8 +772,14 @@
       <c r="S2" s="2">
         <v>18.695070998831401</v>
       </c>
+      <c r="T2">
+        <v>121616</v>
+      </c>
+      <c r="U2">
+        <v>488227</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>235852</v>
       </c>
@@ -819,8 +837,14 @@
       <c r="S3">
         <v>18.482606658193902</v>
       </c>
+      <c r="T3">
+        <v>121613</v>
+      </c>
+      <c r="U3">
+        <v>488215</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>236051</v>
       </c>
@@ -878,8 +902,14 @@
       <c r="S4" s="2">
         <v>12.150798551181801</v>
       </c>
+      <c r="T4">
+        <v>121558</v>
+      </c>
+      <c r="U4">
+        <v>488127</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>236050</v>
       </c>
@@ -937,8 +967,14 @@
       <c r="S5">
         <v>16.3001875513072</v>
       </c>
+      <c r="T5">
+        <v>121558</v>
+      </c>
+      <c r="U5">
+        <v>488117</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>236258</v>
       </c>
@@ -996,8 +1032,14 @@
       <c r="S6" s="2">
         <v>22.718200875125</v>
       </c>
+      <c r="T6">
+        <v>121599</v>
+      </c>
+      <c r="U6">
+        <v>488078</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>236260</v>
       </c>
@@ -1055,8 +1097,14 @@
       <c r="S7" s="2">
         <v>26.612270265710201</v>
       </c>
+      <c r="T7">
+        <v>121608</v>
+      </c>
+      <c r="U7">
+        <v>488071</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>233152</v>
       </c>
@@ -1114,8 +1162,14 @@
       <c r="S8" s="2">
         <v>3</v>
       </c>
+      <c r="T8">
+        <v>121643</v>
+      </c>
+      <c r="U8">
+        <v>488043</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>233386</v>
       </c>
@@ -1173,8 +1227,14 @@
       <c r="S9" s="2">
         <v>28.747853064485099</v>
       </c>
+      <c r="T9">
+        <v>121657</v>
+      </c>
+      <c r="U9">
+        <v>488033</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>233387</v>
       </c>
@@ -1232,8 +1292,14 @@
       <c r="S10" s="2">
         <v>25.587183972678101</v>
       </c>
+      <c r="T10">
+        <v>121667</v>
+      </c>
+      <c r="U10">
+        <v>488026</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>233396</v>
       </c>
@@ -1291,8 +1357,14 @@
       <c r="S11" s="2">
         <v>3</v>
       </c>
+      <c r="T11">
+        <v>121753</v>
+      </c>
+      <c r="U11">
+        <v>487951</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>233624</v>
       </c>
@@ -1350,8 +1422,14 @@
       <c r="S12" s="2">
         <v>33.047994106723799</v>
       </c>
+      <c r="T12">
+        <v>121761</v>
+      </c>
+      <c r="U12">
+        <v>487939</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>224123</v>
       </c>
@@ -1409,8 +1487,14 @@
       <c r="S13" s="2">
         <v>3</v>
       </c>
+      <c r="T13">
+        <v>121819</v>
+      </c>
+      <c r="U13">
+        <v>487739</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>225471</v>
       </c>
@@ -1468,8 +1552,14 @@
       <c r="S14" s="2">
         <v>7.2545081045445698</v>
       </c>
+      <c r="T14">
+        <v>121812</v>
+      </c>
+      <c r="U14">
+        <v>487742</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>223897</v>
       </c>
@@ -1527,8 +1617,14 @@
       <c r="S15" s="2">
         <v>6.3269902368837601</v>
       </c>
+      <c r="T15">
+        <v>121806</v>
+      </c>
+      <c r="U15">
+        <v>487749</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>234320</v>
       </c>
@@ -1586,8 +1682,14 @@
       <c r="S16" s="2">
         <v>21.927299448693699</v>
       </c>
+      <c r="T16">
+        <v>121815</v>
+      </c>
+      <c r="U16">
+        <v>487751</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>234321</v>
       </c>
@@ -1645,8 +1747,14 @@
       <c r="S17" s="2">
         <v>15.6638170953008</v>
       </c>
+      <c r="T17">
+        <v>121825</v>
+      </c>
+      <c r="U17">
+        <v>487752</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>225472</v>
       </c>
@@ -1704,8 +1812,14 @@
       <c r="S18" s="2">
         <v>15.6638170953008</v>
       </c>
+      <c r="T18">
+        <v>121832</v>
+      </c>
+      <c r="U18">
+        <v>487753</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>234318</v>
       </c>
@@ -1763,8 +1877,14 @@
       <c r="S19" s="2">
         <v>13.8642246429247</v>
       </c>
+      <c r="T19">
+        <v>121841</v>
+      </c>
+      <c r="U19">
+        <v>487754</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>234319</v>
       </c>
@@ -1821,6 +1941,12 @@
       </c>
       <c r="S20" s="2">
         <v>21.766103258395699</v>
+      </c>
+      <c r="T20">
+        <v>121853</v>
+      </c>
+      <c r="U20">
+        <v>487755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>